<commit_message>
refactor: Remove internationalization, switch to Chinese-only UI
- Removed the entire internationalization (i18n) system from the project.
- Deleted the `translations` directory and its contents.
- Modified `core/st_utils/sidebar_setting.py`, `st.py`, and `core/st_utils/upload_media_section.py` to replace all `t("key")` calls with hardcoded Chinese strings.
- Removed translation-related imports and UI elements (e.g., display language selector).
- Modified `core/st_utils/imports_and_utils.py` to remove the translation import.
- The UI is now exclusively in Simplified Chinese.
</commit_message>
<xml_diff>
--- a/custom_terms.xlsx
+++ b/custom_terms.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="180">
   <si>
     <t>Source</t>
   </si>
@@ -36,6 +36,537 @@
   </si>
   <si>
     <t>Explain(Optional)</t>
+  </si>
+  <si>
+    <t>ICT</t>
+  </si>
+  <si>
+    <t>market structure shift</t>
+  </si>
+  <si>
+    <t>市场结构转变</t>
+  </si>
+  <si>
+    <t>MSS</t>
+  </si>
+  <si>
+    <t>break of structure</t>
+  </si>
+  <si>
+    <t>结构突破</t>
+  </si>
+  <si>
+    <t>BOS</t>
+  </si>
+  <si>
+    <t>short term high</t>
+  </si>
+  <si>
+    <t>短期高点</t>
+  </si>
+  <si>
+    <t>STH</t>
+  </si>
+  <si>
+    <t>short term low</t>
+  </si>
+  <si>
+    <t>短期低点</t>
+  </si>
+  <si>
+    <t>STL</t>
+  </si>
+  <si>
+    <t>intermediate term high</t>
+  </si>
+  <si>
+    <t>中期高点</t>
+  </si>
+  <si>
+    <t>ITH</t>
+  </si>
+  <si>
+    <t>intermediate term low</t>
+  </si>
+  <si>
+    <t>中期低点</t>
+  </si>
+  <si>
+    <t>ITL</t>
+  </si>
+  <si>
+    <t>long term high</t>
+  </si>
+  <si>
+    <t>长期高点</t>
+  </si>
+  <si>
+    <t>LTH</t>
+  </si>
+  <si>
+    <t>long term low</t>
+  </si>
+  <si>
+    <t>长期低点</t>
+  </si>
+  <si>
+    <t>LTL</t>
+  </si>
+  <si>
+    <t>buy-side liquidity</t>
+  </si>
+  <si>
+    <t>买方流动性</t>
+  </si>
+  <si>
+    <t>BSL</t>
+  </si>
+  <si>
+    <t>sell-side liquidity</t>
+  </si>
+  <si>
+    <t>卖方流动性</t>
+  </si>
+  <si>
+    <t>SSL</t>
+  </si>
+  <si>
+    <t>relatively equal highs</t>
+  </si>
+  <si>
+    <t>相对等高点</t>
+  </si>
+  <si>
+    <t>REH</t>
+  </si>
+  <si>
+    <t>relatively equal lows</t>
+  </si>
+  <si>
+    <t>相对等低点</t>
+  </si>
+  <si>
+    <t>REL</t>
+  </si>
+  <si>
+    <t>previous day high</t>
+  </si>
+  <si>
+    <t>前一天高点</t>
+  </si>
+  <si>
+    <t>PDH</t>
+  </si>
+  <si>
+    <t>previous day low</t>
+  </si>
+  <si>
+    <t>前一天低点</t>
+  </si>
+  <si>
+    <t>PDL</t>
+  </si>
+  <si>
+    <t>previous week high</t>
+  </si>
+  <si>
+    <t>前一周高点</t>
+  </si>
+  <si>
+    <t>PWH</t>
+  </si>
+  <si>
+    <t>previous week low</t>
+  </si>
+  <si>
+    <t>前一周低点</t>
+  </si>
+  <si>
+    <t>PWL</t>
+  </si>
+  <si>
+    <t>inducement</t>
+  </si>
+  <si>
+    <t>诱因</t>
+  </si>
+  <si>
+    <t>IDM</t>
+  </si>
+  <si>
+    <t>fair value gap</t>
+  </si>
+  <si>
+    <t>公允价值缺口</t>
+  </si>
+  <si>
+    <t>FVG</t>
+  </si>
+  <si>
+    <t>buy-side imbalance</t>
+  </si>
+  <si>
+    <t>买方失衡</t>
+  </si>
+  <si>
+    <t>sell-side inefficiency</t>
+  </si>
+  <si>
+    <t>卖方低效</t>
+  </si>
+  <si>
+    <t>sell-side imbalance</t>
+  </si>
+  <si>
+    <t>卖方失衡</t>
+  </si>
+  <si>
+    <t>buy-side inefficiency</t>
+  </si>
+  <si>
+    <t>买方低效</t>
+  </si>
+  <si>
+    <t>order block</t>
+  </si>
+  <si>
+    <t>订单块</t>
+  </si>
+  <si>
+    <t>OB</t>
+  </si>
+  <si>
+    <t>breaker block/breaker</t>
+  </si>
+  <si>
+    <t>突破块</t>
+  </si>
+  <si>
+    <t>BB</t>
+  </si>
+  <si>
+    <t>mitigation block</t>
+  </si>
+  <si>
+    <t>缓解块</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>rejection block</t>
+  </si>
+  <si>
+    <t>拒绝块</t>
+  </si>
+  <si>
+    <t>RB</t>
+  </si>
+  <si>
+    <t>volume imbalance</t>
+  </si>
+  <si>
+    <t>成交量失衡</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>market maker buy model</t>
+  </si>
+  <si>
+    <t>做市商买入模型</t>
+  </si>
+  <si>
+    <t>MMBM</t>
+  </si>
+  <si>
+    <t>market maker sell model</t>
+  </si>
+  <si>
+    <t>做市商卖出模型</t>
+  </si>
+  <si>
+    <t>MMSM</t>
+  </si>
+  <si>
+    <t>consequent encroachment</t>
+  </si>
+  <si>
+    <t>缺口中点</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>mean threshold</t>
+  </si>
+  <si>
+    <t>均值阈值</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>smart money technique</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>术语不译</t>
+  </si>
+  <si>
+    <t>institutional order flow</t>
+  </si>
+  <si>
+    <t>机构订单流</t>
+  </si>
+  <si>
+    <t>IOF</t>
+  </si>
+  <si>
+    <t>draw on liquidity</t>
+  </si>
+  <si>
+    <t>流动性吸引</t>
+  </si>
+  <si>
+    <t>DOL</t>
+  </si>
+  <si>
+    <t>point of interest</t>
+  </si>
+  <si>
+    <t>POI</t>
+  </si>
+  <si>
+    <t>power of three</t>
+  </si>
+  <si>
+    <t>PO3</t>
+  </si>
+  <si>
+    <t>accumulation</t>
+  </si>
+  <si>
+    <t>盘整</t>
+  </si>
+  <si>
+    <t>manipulation</t>
+  </si>
+  <si>
+    <t>操纵</t>
+  </si>
+  <si>
+    <t>distribution</t>
+  </si>
+  <si>
+    <t>派发</t>
+  </si>
+  <si>
+    <t>optimal trade entry</t>
+  </si>
+  <si>
+    <t>最佳交易入场点</t>
+  </si>
+  <si>
+    <t>OTE</t>
+  </si>
+  <si>
+    <t>midnight opening price</t>
+  </si>
+  <si>
+    <t>午夜开盘价</t>
+  </si>
+  <si>
+    <t>MOP</t>
+  </si>
+  <si>
+    <t>higher time frame</t>
+  </si>
+  <si>
+    <t>高时间周期</t>
+  </si>
+  <si>
+    <t>HTF</t>
+  </si>
+  <si>
+    <t>lower time frame</t>
+  </si>
+  <si>
+    <t>低时间周期</t>
+  </si>
+  <si>
+    <t>LTF</t>
+  </si>
+  <si>
+    <t>standard deviation</t>
+  </si>
+  <si>
+    <t>标准差</t>
+  </si>
+  <si>
+    <t>STDV</t>
+  </si>
+  <si>
+    <t>open high low close</t>
+  </si>
+  <si>
+    <t>OHLC</t>
+  </si>
+  <si>
+    <t>london open kill zone</t>
+  </si>
+  <si>
+    <t>伦敦开盘杀戮区</t>
+  </si>
+  <si>
+    <t>LOKZ</t>
+  </si>
+  <si>
+    <t>london close kill zone</t>
+  </si>
+  <si>
+    <t>伦敦收盘杀戮区</t>
+  </si>
+  <si>
+    <t>LCKZ</t>
+  </si>
+  <si>
+    <t>new york open kill zone</t>
+  </si>
+  <si>
+    <t>纽约开盘杀戮区</t>
+  </si>
+  <si>
+    <t>NYOKZ</t>
+  </si>
+  <si>
+    <t>PD Array</t>
+  </si>
+  <si>
+    <t>PD 区域</t>
+  </si>
+  <si>
+    <t>premium</t>
+  </si>
+  <si>
+    <t>溢价</t>
+  </si>
+  <si>
+    <t>discount</t>
+  </si>
+  <si>
+    <t>折价</t>
+  </si>
+  <si>
+    <t>stop hunt</t>
+  </si>
+  <si>
+    <t>止损猎杀</t>
+  </si>
+  <si>
+    <t>liquidity pool</t>
+  </si>
+  <si>
+    <t>流动性池</t>
+  </si>
+  <si>
+    <t>BPR</t>
+  </si>
+  <si>
+    <t>价格平衡区间</t>
+  </si>
+  <si>
+    <t>swing low</t>
+  </si>
+  <si>
+    <t>摆动低点</t>
+  </si>
+  <si>
+    <t>swing high</t>
+  </si>
+  <si>
+    <t>摆动高点</t>
+  </si>
+  <si>
+    <t>daily bias</t>
+  </si>
+  <si>
+    <t>每日偏见</t>
+  </si>
+  <si>
+    <t>bias</t>
+  </si>
+  <si>
+    <t>偏见</t>
+  </si>
+  <si>
+    <t>double purge</t>
+  </si>
+  <si>
+    <t>双重清洗</t>
+  </si>
+  <si>
+    <t>failure swing</t>
+  </si>
+  <si>
+    <t>失败摆动</t>
+  </si>
+  <si>
+    <t>ment blocks</t>
+  </si>
+  <si>
+    <t>MBs</t>
+  </si>
+  <si>
+    <t>mentfx block</t>
+  </si>
+  <si>
+    <t>validated Ment block</t>
+  </si>
+  <si>
+    <t>已验证 MB</t>
+  </si>
+  <si>
+    <t>bullish Ment block</t>
+  </si>
+  <si>
+    <t>看涨 MB</t>
+  </si>
+  <si>
+    <t>EVC</t>
+  </si>
+  <si>
+    <t>EV</t>
+  </si>
+  <si>
+    <t>Axis Circle</t>
+  </si>
+  <si>
+    <t>Axis system</t>
+  </si>
+  <si>
+    <t>Axis 系统</t>
+  </si>
+  <si>
+    <t>expansion</t>
+  </si>
+  <si>
+    <t>扩张</t>
+  </si>
+  <si>
+    <t>Marcell</t>
+  </si>
+  <si>
+    <t>minus 0.27</t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>积累-操纵-派发</t>
   </si>
 </sst>
 </file>
@@ -912,7 +1443,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{CB3BB329-D340-4F11-B6F6-6CD85F254356}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{B28E39D7-8B71-462F-9B49-CD05319B4065}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -921,7 +1452,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{F5927B29-E009-4E28-B5F3-180F4A9AB80C}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{9C348754-8554-434C-A731-D7D1FFCDE705}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1152,10 +1683,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C75" sqref="C75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81666666666667" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -1177,6 +1708,739 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" t="s">
+        <v>78</v>
+      </c>
+      <c r="B29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C29" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" t="s">
+        <v>81</v>
+      </c>
+      <c r="B30" t="s">
+        <v>82</v>
+      </c>
+      <c r="C30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" t="s">
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>85</v>
+      </c>
+      <c r="C31" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" t="s">
+        <v>99</v>
+      </c>
+      <c r="B36" t="s">
+        <v>100</v>
+      </c>
+      <c r="C36" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" t="s">
+        <v>102</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="C37" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>110</v>
+      </c>
+      <c r="B41" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C42" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" t="s">
+        <v>115</v>
+      </c>
+      <c r="B43" t="s">
+        <v>116</v>
+      </c>
+      <c r="C43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" t="s">
+        <v>118</v>
+      </c>
+      <c r="B44" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" t="s">
+        <v>121</v>
+      </c>
+      <c r="B45" t="s">
+        <v>122</v>
+      </c>
+      <c r="C45" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+      <c r="C46" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" t="s">
+        <v>128</v>
+      </c>
+      <c r="C47" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="C48" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="C49" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="C50" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>140</v>
+      </c>
+      <c r="B52" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>142</v>
+      </c>
+      <c r="B53" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>146</v>
+      </c>
+      <c r="B55" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>148</v>
+      </c>
+      <c r="B56" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>150</v>
+      </c>
+      <c r="B57" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>152</v>
+      </c>
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>154</v>
+      </c>
+      <c r="B59" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>156</v>
+      </c>
+      <c r="B60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>158</v>
+      </c>
+      <c r="B61" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>160</v>
+      </c>
+      <c r="B62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" t="s">
+        <v>162</v>
+      </c>
+      <c r="B63" t="s">
+        <v>163</v>
+      </c>
+      <c r="C63" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3">
+      <c r="A64" t="s">
+        <v>164</v>
+      </c>
+      <c r="B64" t="s">
+        <v>74</v>
+      </c>
+      <c r="C64" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>74</v>
+      </c>
+      <c r="B65" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>165</v>
+      </c>
+      <c r="B66" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>167</v>
+      </c>
+      <c r="B67" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>169</v>
+      </c>
+      <c r="B68" t="s">
+        <v>169</v>
+      </c>
+      <c r="C68" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>170</v>
+      </c>
+      <c r="B69" t="s">
+        <v>170</v>
+      </c>
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>171</v>
+      </c>
+      <c r="B70" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>172</v>
+      </c>
+      <c r="B71" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>174</v>
+      </c>
+      <c r="B72" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>176</v>
+      </c>
+      <c r="B73" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>177</v>
+      </c>
+      <c r="B74">
+        <v>-0.27</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" t="s">
+        <v>178</v>
+      </c>
+      <c r="B75" t="s">
+        <v>178</v>
+      </c>
+      <c r="C75" t="s">
+        <v>179</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="600" verticalDpi="600"/>

</xml_diff>

<commit_message>
fix: clear custom_terms.xlsx to empty template
🤖 Generated with [Claude Code](https://claude.com/claude-code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/custom_terms.xlsx
+++ b/custom_terms.xlsx
@@ -912,7 +912,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="2" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{AD434D0A-1DF6-4BFD-B31D-182FFE0870D8}">
+    <tableStyle name="TableStylePreset3_Accent1 1" pivot="0" count="7" xr9:uid="{EAB357E5-A241-44C6-9C66-41DE39CAD877}">
       <tableStyleElement type="wholeTable" dxfId="6"/>
       <tableStyleElement type="headerRow" dxfId="5"/>
       <tableStyleElement type="totalRow" dxfId="4"/>
@@ -921,7 +921,7 @@
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="firstColumnStripe" dxfId="0"/>
     </tableStyle>
-    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{6C1C25F5-422A-482F-9536-03B625A6A853}">
+    <tableStyle name="PivotStylePreset2_Accent1 1" table="0" count="10" xr9:uid="{F8FE5F0E-0DD6-4BA4-9C60-EBE7B1A31797}">
       <tableStyleElement type="headerRow" dxfId="16"/>
       <tableStyleElement type="totalRow" dxfId="15"/>
       <tableStyleElement type="firstRowStripe" dxfId="14"/>
@@ -1154,8 +1154,8 @@
   <sheetPr/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A75" sqref="$A2:$XFD75"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.81666666666667" defaultRowHeight="14.25" outlineLevelCol="2"/>

</xml_diff>